<commit_message>
Cuaderno de estudio CS_11_01
con los ajustes de escaleta pedidos por el autor. Falta ver si los
cambios de imágenes no modificarán el texto de manuscrito
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/ESCALETA_CS_11_01_CO - agosto 22.xlsx
+++ b/fuentes/contenidos/grado11/guion01/ESCALETA_CS_11_01_CO - agosto 22.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flor\Dropbox\EdPlaneta - autores CS-11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flor\Documents\Trabajo Ed Planeta\CienciasSociales\fuentes\contenidos\grado11\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="264">
   <si>
     <t>Asignatura</t>
   </si>
@@ -878,6 +878,9 @@
   </si>
   <si>
     <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>Actividad sobre Los conflictos en Medio Oriente</t>
   </si>
 </sst>
 </file>
@@ -1080,48 +1083,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1253,6 +1214,48 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3526,2450 +3529,2452 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="51" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="52" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="53" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="31" customWidth="1"/>
-    <col min="7" max="7" width="41.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="56" customWidth="1"/>
-    <col min="10" max="10" width="60" style="26" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="59" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="45.42578125" style="27" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="28" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="37" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" style="33" customWidth="1"/>
-    <col min="22" max="16384" width="11.42578125" style="17"/>
+    <col min="1" max="1" width="15" style="37" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="39" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="42" customWidth="1"/>
+    <col min="10" max="10" width="60" style="12" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="45.42578125" style="13" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" style="14" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="23" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="19" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="13" t="s">
+      <c r="N1" s="54"/>
+      <c r="O1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="49" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="18" t="s">
+      <c r="A2" s="53"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="15"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="43">
         <v>1</v>
       </c>
-      <c r="I3" s="55" t="s">
+      <c r="I3" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="58" t="s">
+      <c r="L3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="58" t="s">
+      <c r="M3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="58"/>
-      <c r="P3" s="28" t="s">
+      <c r="N3" s="44"/>
+      <c r="P3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="37">
+      <c r="Q3" s="23">
         <v>6</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="R3" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="S3" s="33" t="s">
+      <c r="S3" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="T3" s="54" t="s">
+      <c r="T3" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="U3" s="33" t="s">
+      <c r="U3" s="19" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="16" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="55"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="41"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
     </row>
     <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="21">
         <v>2</v>
       </c>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="K6" s="58" t="s">
+      <c r="K6" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="58" t="s">
+      <c r="L6" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58" t="s">
+      <c r="M6" s="44"/>
+      <c r="N6" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="36" t="s">
+      <c r="O6" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="P6" s="28" t="s">
+      <c r="P6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="37">
+      <c r="Q6" s="23">
         <v>6</v>
       </c>
-      <c r="R6" s="38" t="s">
+      <c r="R6" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S6" s="39" t="s">
+      <c r="S6" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T6" s="40" t="s">
+      <c r="T6" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="U6" s="39" t="s">
+      <c r="U6" s="25" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="21">
         <v>3</v>
       </c>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="K7" s="58" t="s">
+      <c r="K7" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="58" t="s">
+      <c r="L7" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58" t="s">
+      <c r="M7" s="44"/>
+      <c r="N7" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="O7" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="P7" s="28" t="s">
+      <c r="P7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="37">
+      <c r="Q7" s="23">
         <v>6</v>
       </c>
-      <c r="R7" s="38" t="s">
+      <c r="R7" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S7" s="39" t="s">
+      <c r="S7" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T7" s="40" t="s">
+      <c r="T7" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="U7" s="39" t="s">
+      <c r="U7" s="25" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="21">
         <v>4</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="K8" s="58" t="s">
+      <c r="K8" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="58" t="s">
+      <c r="L8" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="58" t="s">
+      <c r="M8" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="N8" s="58"/>
-      <c r="P8" s="28" t="s">
+      <c r="N8" s="44"/>
+      <c r="P8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="37">
+      <c r="Q8" s="23">
         <v>6</v>
       </c>
-      <c r="R8" s="38" t="s">
+      <c r="R8" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="S8" s="33" t="s">
+      <c r="S8" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="T8" s="54" t="s">
+      <c r="T8" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="U8" s="33" t="s">
+      <c r="U8" s="19" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="55"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="41"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
     </row>
     <row r="10" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="55"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="41"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
     </row>
     <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="21">
         <v>5</v>
       </c>
-      <c r="I11" s="55" t="s">
+      <c r="I11" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="K11" s="58" t="s">
+      <c r="K11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="L11" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="58" t="s">
+      <c r="N11" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="23">
         <v>6</v>
       </c>
-      <c r="R11" s="38" t="s">
+      <c r="R11" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S11" s="33" t="s">
+      <c r="S11" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="T11" s="54" t="s">
+      <c r="T11" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="U11" s="33" t="s">
+      <c r="U11" s="19" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H12" s="21">
         <v>6</v>
       </c>
-      <c r="I12" s="55" t="s">
+      <c r="I12" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="K12" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="58" t="s">
+      <c r="L12" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58" t="s">
+      <c r="M12" s="44"/>
+      <c r="N12" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="41" t="s">
+      <c r="O12" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="P12" s="28" t="s">
+      <c r="P12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="37">
+      <c r="Q12" s="23">
         <v>6</v>
       </c>
-      <c r="R12" s="38" t="s">
+      <c r="R12" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S12" s="39" t="s">
+      <c r="S12" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T12" s="40" t="s">
+      <c r="T12" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="U12" s="39" t="s">
+      <c r="U12" s="25" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="21">
         <v>7</v>
       </c>
-      <c r="I13" s="55" t="s">
+      <c r="I13" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="58" t="s">
+      <c r="L13" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="58" t="s">
+      <c r="M13" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="N13" s="58"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="28" t="s">
+      <c r="N13" s="44"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="37">
+      <c r="Q13" s="23">
         <v>6</v>
       </c>
-      <c r="R13" s="38" t="s">
+      <c r="R13" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="S13" s="39" t="s">
+      <c r="S13" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="T13" s="40" t="s">
+      <c r="T13" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="U13" s="39" t="s">
+      <c r="U13" s="25" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="55"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="41"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
     </row>
     <row r="15" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="55"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="41"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
     </row>
     <row r="16" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="G16" s="34" t="s">
+      <c r="G16" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="35">
+      <c r="H16" s="21">
         <v>8</v>
       </c>
-      <c r="I16" s="55" t="s">
+      <c r="I16" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="34" t="s">
+      <c r="J16" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="K16" s="58" t="s">
+      <c r="K16" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="58" t="s">
+      <c r="L16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="58"/>
-      <c r="N16" s="58" t="s">
+      <c r="M16" s="44"/>
+      <c r="N16" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="36" t="s">
+      <c r="O16" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="P16" s="28" t="s">
+      <c r="P16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="37">
+      <c r="Q16" s="23">
         <v>6</v>
       </c>
-      <c r="R16" s="38" t="s">
+      <c r="R16" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S16" s="39" t="s">
+      <c r="S16" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T16" s="40" t="s">
+      <c r="T16" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="U16" s="39" t="s">
+      <c r="U16" s="25" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="55"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="41"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="44"/>
     </row>
     <row r="18" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="55"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="41"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
     </row>
     <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="55"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="41"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="44"/>
     </row>
     <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="36"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="40"/>
-      <c r="U20" s="39"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="22"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="25"/>
     </row>
     <row r="21" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="55"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="41"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="G22" s="34" t="s">
+      <c r="G22" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="H22" s="35">
+      <c r="H22" s="21">
         <v>9</v>
       </c>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="K22" s="58" t="s">
+      <c r="K22" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="58" t="s">
+      <c r="L22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58" t="s">
+      <c r="M22" s="44"/>
+      <c r="N22" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="O22" s="41" t="s">
+      <c r="O22" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="P22" s="28" t="s">
+      <c r="P22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="37">
+      <c r="Q22" s="23">
         <v>6</v>
       </c>
-      <c r="R22" s="38" t="s">
+      <c r="R22" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S22" s="39" t="s">
+      <c r="S22" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T22" s="40" t="s">
+      <c r="T22" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="U22" s="39" t="s">
+      <c r="U22" s="25" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="55"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
-      <c r="N23" s="58"/>
-    </row>
-    <row r="24" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="41"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+    </row>
+    <row r="24" spans="1:21" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44" t="s">
+      <c r="F24" s="29"/>
+      <c r="G24" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="H24" s="35">
+      <c r="H24" s="21">
         <v>10</v>
       </c>
-      <c r="I24" s="57" t="s">
+      <c r="I24" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="45" t="s">
+      <c r="J24" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="K24" s="60" t="s">
+      <c r="K24" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="60" t="s">
+      <c r="L24" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M24" s="60" t="s">
+      <c r="M24" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="60"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="46" t="s">
+      <c r="N24" s="46"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="37">
+      <c r="Q24" s="23">
         <v>6</v>
       </c>
-      <c r="R24" s="38" t="s">
+      <c r="R24" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="S24" s="39" t="s">
+      <c r="S24" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="T24" s="40" t="s">
+      <c r="T24" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="U24" s="39" t="s">
+      <c r="U24" s="25" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="G25" s="44" t="s">
+      <c r="G25" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="H25" s="35">
+      <c r="H25" s="21">
         <v>11</v>
       </c>
-      <c r="I25" s="55" t="s">
+      <c r="I25" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="K25" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="O25" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="P25" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="K25" s="58" t="s">
+      <c r="Q25" s="23">
+        <v>6</v>
+      </c>
+      <c r="R25" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="S25" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="T25" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="U25" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="H26" s="21">
+        <v>12</v>
+      </c>
+      <c r="I26" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="O25" s="36" t="s">
-        <v>172</v>
-      </c>
-      <c r="P25" s="28" t="s">
+      <c r="J26" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="K26" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="O26" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="P26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="37">
+      <c r="Q26" s="23">
         <v>6</v>
       </c>
-      <c r="R25" s="38" t="s">
+      <c r="R26" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S25" s="33" t="s">
+      <c r="S26" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T25" s="54" t="s">
-        <v>213</v>
-      </c>
-      <c r="U25" s="33" t="s">
+      <c r="T26" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="U26" s="25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+    <row r="27" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B27" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C27" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="E26" s="30" t="s">
+      <c r="D27" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="I27" s="41"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+    </row>
+    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="H28" s="21">
+        <v>13</v>
+      </c>
+      <c r="I28" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="K28" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="O28" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="P28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q28" s="23">
+        <v>6</v>
+      </c>
+      <c r="R28" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="S28" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="T28" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="U28" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="I29" s="41"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+    </row>
+    <row r="30" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="41"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+    </row>
+    <row r="31" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="H31" s="21">
+        <v>14</v>
+      </c>
+      <c r="I31" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="K31" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="O31" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="P31" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q31" s="23">
+        <v>6</v>
+      </c>
+      <c r="R31" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="S31" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="T31" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="U31" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="I32" s="41"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="44"/>
+    </row>
+    <row r="33" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E33" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="G26" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="H26" s="35">
-        <v>12</v>
-      </c>
-      <c r="I26" s="55" t="s">
+      <c r="G33" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="H33" s="21">
+        <v>15</v>
+      </c>
+      <c r="I33" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="K26" s="58" t="s">
+      <c r="J33" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="K33" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="58" t="s">
+      <c r="L33" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58" t="s">
+      <c r="M33" s="44"/>
+      <c r="N33" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="O26" s="41" t="s">
+      <c r="O33" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="P26" s="28" t="s">
+      <c r="P33" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="37">
+      <c r="Q33" s="23">
         <v>6</v>
       </c>
-      <c r="R26" s="38" t="s">
+      <c r="R33" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S26" s="39" t="s">
+      <c r="S33" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T26" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="U26" s="39" t="s">
+      <c r="T33" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="U33" s="25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+    <row r="34" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B34" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C34" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="I27" s="55"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-    </row>
-    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="D34" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H34" s="21">
+        <v>16</v>
+      </c>
+      <c r="I34" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="K34" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="M34" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="N34" s="44"/>
+      <c r="Q34" s="23">
+        <v>6</v>
+      </c>
+      <c r="R34" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="S34" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="T34" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="U34" s="19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B35" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C35" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="H28" s="35">
-        <v>13</v>
-      </c>
-      <c r="I28" s="55" t="s">
+      <c r="D35" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
+    </row>
+    <row r="36" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" s="21">
+        <v>17</v>
+      </c>
+      <c r="I36" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="K28" s="58" t="s">
+      <c r="J36" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="K36" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="58" t="s">
+      <c r="L36" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58" t="s">
+      <c r="M36" s="44"/>
+      <c r="N36" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="O28" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="P28" s="28" t="s">
+      <c r="O36" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="P36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="37">
+      <c r="Q36" s="23">
         <v>6</v>
       </c>
-      <c r="R28" s="38" t="s">
+      <c r="R36" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S28" s="39" t="s">
+      <c r="S36" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T28" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="U28" s="39" t="s">
+      <c r="T36" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="U36" s="25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+    <row r="37" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B37" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C37" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="I29" s="55"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="58"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="58"/>
-    </row>
-    <row r="30" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="D37" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="G37" s="20"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="44"/>
+      <c r="S37" s="25"/>
+      <c r="T37" s="35"/>
+      <c r="U37" s="25"/>
+    </row>
+    <row r="38" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B38" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C38" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D30" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="F30" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="G30" s="34"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="55"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-    </row>
-    <row r="31" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="D38" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="H38" s="21">
         <v>18</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="I38" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="K38" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M38" s="44"/>
+      <c r="N38" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="O38" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="P38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q38" s="23">
+        <v>6</v>
+      </c>
+      <c r="R38" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="S38" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="T38" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="U38" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C39" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="H31" s="35">
-        <v>14</v>
-      </c>
-      <c r="I31" s="55" t="s">
+      <c r="D39" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="H39" s="21">
+        <v>19</v>
+      </c>
+      <c r="I39" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="K39" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="K31" s="58" t="s">
+      <c r="L39" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="M39" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="N39" s="44"/>
+      <c r="Q39" s="23">
+        <v>6</v>
+      </c>
+      <c r="R39" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="S39" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="T39" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="U39" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="44"/>
+      <c r="N40" s="44"/>
+      <c r="S40" s="25"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="25"/>
+    </row>
+    <row r="41" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="H41" s="21">
         <v>20</v>
       </c>
-      <c r="L31" s="58" t="s">
+      <c r="I41" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="K41" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L41" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="O31" s="41" t="s">
+      <c r="M41" s="44"/>
+      <c r="N41" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="P41" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q41" s="23">
+        <v>6</v>
+      </c>
+      <c r="R41" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="S41" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="T41" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="U41" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="I42" s="41"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44"/>
+    </row>
+    <row r="43" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="H43" s="21">
+        <v>21</v>
+      </c>
+      <c r="I43" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="K43" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="O43" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="P43" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q43" s="23">
+        <v>6</v>
+      </c>
+      <c r="R43" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="S43" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="T43" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="U43" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="I44" s="41"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44"/>
+    </row>
+    <row r="45" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H45" s="21">
+        <v>22</v>
+      </c>
+      <c r="I45" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="K45" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M45" s="44"/>
+      <c r="N45" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="O45" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="P31" s="28" t="s">
+      <c r="P45" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="37">
+      <c r="Q45" s="23">
         <v>6</v>
       </c>
-      <c r="R31" s="38" t="s">
+      <c r="R45" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S31" s="39" t="s">
+      <c r="S45" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T31" s="40" t="s">
-        <v>214</v>
-      </c>
-      <c r="U31" s="39" t="s">
+      <c r="T45" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="U45" s="25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+    <row r="46" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B46" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C46" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="I32" s="55"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-    </row>
-    <row r="33" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="D46" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="G46" s="20"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="41"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="44"/>
+    </row>
+    <row r="47" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B47" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C47" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="G33" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="H33" s="35">
-        <v>15</v>
-      </c>
-      <c r="I33" s="55" t="s">
+      <c r="D47" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="H47" s="21">
+        <v>23</v>
+      </c>
+      <c r="I47" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="K47" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="48" t="s">
-        <v>199</v>
-      </c>
-      <c r="K33" s="58" t="s">
+      <c r="L47" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="N47" s="44"/>
+      <c r="O47" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="P47" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q47" s="23">
+        <v>6</v>
+      </c>
+      <c r="R47" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="S47" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="T47" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="U47" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H48" s="21">
+        <v>24</v>
+      </c>
+      <c r="I48" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="L33" s="58" t="s">
+      <c r="J48" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="K48" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="O33" s="41" t="s">
+      <c r="M48" s="44"/>
+      <c r="N48" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="O48" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="P33" s="28" t="s">
+      <c r="P48" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="37">
+      <c r="Q48" s="23">
         <v>6</v>
       </c>
-      <c r="R33" s="38" t="s">
+      <c r="R48" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S33" s="39" t="s">
+      <c r="S48" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T33" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="U33" s="39" t="s">
+      <c r="T48" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="U48" s="25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+    <row r="49" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B49" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C49" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="G34" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="H34" s="35">
-        <v>16</v>
-      </c>
-      <c r="I34" s="55" t="s">
+      <c r="D49" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="I49" s="41"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="44"/>
+      <c r="N49" s="44"/>
+      <c r="S49" s="25"/>
+      <c r="T49" s="35"/>
+      <c r="U49" s="25"/>
+    </row>
+    <row r="50" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="21">
+        <v>25</v>
+      </c>
+      <c r="I50" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="K50" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L50" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="M50" s="44"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="27"/>
+      <c r="P50" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J34" s="48" t="s">
-        <v>201</v>
-      </c>
-      <c r="K34" s="58" t="s">
+      <c r="S50" s="25"/>
+      <c r="T50" s="26"/>
+      <c r="U50" s="25"/>
+    </row>
+    <row r="51" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="H51" s="21">
+        <v>26</v>
+      </c>
+      <c r="I51" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="L34" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="M34" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="N34" s="58"/>
-      <c r="Q34" s="37">
+      <c r="J51" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="K51" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M51" s="44"/>
+      <c r="N51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="O51" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="P51" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q51" s="23">
         <v>6</v>
       </c>
-      <c r="R34" s="38" t="s">
+      <c r="R51" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S34" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="T34" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="U34" s="33" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="S51" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="T51" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="U51" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B52" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C52" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D35" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="G35" s="34"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-    </row>
-    <row r="36" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="D52" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="I52" s="41"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="44"/>
+      <c r="M52" s="44"/>
+      <c r="N52" s="44"/>
+      <c r="O52" s="27"/>
+      <c r="S52" s="25"/>
+      <c r="T52" s="35"/>
+      <c r="U52" s="25"/>
+    </row>
+    <row r="53" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B53" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C53" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="H36" s="35">
-        <v>17</v>
-      </c>
-      <c r="I36" s="55" t="s">
+      <c r="D53" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G53" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="H53" s="21">
+        <v>27</v>
+      </c>
+      <c r="I53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="K36" s="58" t="s">
+      <c r="J53" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="K53" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L36" s="58" t="s">
+      <c r="L53" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="O36" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="P36" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q36" s="37">
+      <c r="M53" s="44"/>
+      <c r="N53" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="O53" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="P53" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q53" s="23">
         <v>6</v>
       </c>
-      <c r="R36" s="38" t="s">
+      <c r="R53" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="S36" s="39" t="s">
+      <c r="S53" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T36" s="40" t="s">
-        <v>218</v>
-      </c>
-      <c r="U36" s="39" t="s">
+      <c r="T53" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="U53" s="25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="G37" s="34"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="S37" s="39"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="39"/>
-    </row>
-    <row r="38" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="G38" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="H38" s="35">
-        <v>18</v>
-      </c>
-      <c r="I38" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J38" s="48"/>
-      <c r="K38" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="M38" s="58"/>
-      <c r="N38" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="O38" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="P38" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q38" s="37">
-        <v>6</v>
-      </c>
-      <c r="R38" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="S38" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="T38" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="U38" s="39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="G39" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="H39" s="35">
-        <v>19</v>
-      </c>
-      <c r="I39" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="J39" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="K39" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="M39" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="N39" s="58"/>
-      <c r="Q39" s="37">
-        <v>6</v>
-      </c>
-      <c r="R39" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="S39" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="T39" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="U39" s="33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>256</v>
-      </c>
-      <c r="G40" s="34"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="58"/>
-      <c r="L40" s="58"/>
-      <c r="M40" s="58"/>
-      <c r="N40" s="58"/>
-      <c r="S40" s="39"/>
-      <c r="T40" s="49"/>
-      <c r="U40" s="39"/>
-    </row>
-    <row r="41" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="G41" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="H41" s="35">
-        <v>20</v>
-      </c>
-      <c r="I41" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J41" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="K41" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="M41" s="58"/>
-      <c r="N41" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="P41" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q41" s="37">
-        <v>6</v>
-      </c>
-      <c r="R41" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="S41" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="T41" s="54" t="s">
-        <v>220</v>
-      </c>
-      <c r="U41" s="33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="E42" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="G42" s="34"/>
-      <c r="I42" s="55"/>
-      <c r="K42" s="58"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58"/>
-    </row>
-    <row r="43" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="F43" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="G43" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="H43" s="35">
-        <v>21</v>
-      </c>
-      <c r="I43" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J43" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="K43" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L43" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="O43" s="50" t="s">
-        <v>179</v>
-      </c>
-      <c r="P43" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q43" s="37">
-        <v>6</v>
-      </c>
-      <c r="R43" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="S43" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="T43" s="40" t="s">
-        <v>180</v>
-      </c>
-      <c r="U43" s="39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>259</v>
-      </c>
-      <c r="I44" s="55"/>
-      <c r="K44" s="58"/>
-      <c r="L44" s="58"/>
-      <c r="M44" s="58"/>
-      <c r="N44" s="58"/>
-    </row>
-    <row r="45" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="G45" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="H45" s="35">
-        <v>22</v>
-      </c>
-      <c r="I45" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J45" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="K45" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L45" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="M45" s="58"/>
-      <c r="N45" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="O45" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="P45" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q45" s="37">
-        <v>6</v>
-      </c>
-      <c r="R45" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="S45" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="T45" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="U45" s="39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="G46" s="34"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="55"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-    </row>
-    <row r="47" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="G47" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="H47" s="35">
-        <v>23</v>
-      </c>
-      <c r="I47" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="J47" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="K47" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L47" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="M47" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="N47" s="58"/>
-      <c r="O47" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="P47" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q47" s="37">
-        <v>6</v>
-      </c>
-      <c r="R47" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="S47" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="T47" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="U47" s="39" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="G48" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H48" s="35">
-        <v>24</v>
-      </c>
-      <c r="I48" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J48" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="K48" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="O48" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="P48" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q48" s="37">
-        <v>6</v>
-      </c>
-      <c r="R48" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="S48" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="T48" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="U48" s="39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="I49" s="55"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="S49" s="39"/>
-      <c r="T49" s="49"/>
-      <c r="U49" s="39"/>
-    </row>
-    <row r="50" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="35">
-        <v>25</v>
-      </c>
-      <c r="I50" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J50" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="K50" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L50" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="41"/>
-      <c r="P50" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="S50" s="39"/>
-      <c r="T50" s="40"/>
-      <c r="U50" s="39"/>
-    </row>
-    <row r="51" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="E51" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="G51" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="H51" s="35">
-        <v>26</v>
-      </c>
-      <c r="I51" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J51" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="K51" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="M51" s="58"/>
-      <c r="N51" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="O51" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="P51" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q51" s="37">
-        <v>6</v>
-      </c>
-      <c r="R51" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="S51" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="T51" s="40" t="s">
-        <v>222</v>
-      </c>
-      <c r="U51" s="39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D52" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="E52" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I52" s="55"/>
-      <c r="K52" s="58"/>
-      <c r="L52" s="58"/>
-      <c r="M52" s="58"/>
-      <c r="N52" s="58"/>
-      <c r="O52" s="41"/>
-      <c r="S52" s="39"/>
-      <c r="T52" s="49"/>
-      <c r="U52" s="39"/>
-    </row>
-    <row r="53" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D53" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="G53" s="44" t="s">
-        <v>188</v>
-      </c>
-      <c r="H53" s="35">
-        <v>27</v>
-      </c>
-      <c r="I53" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J53" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="K53" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L53" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="M53" s="58"/>
-      <c r="N53" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="O53" s="41" t="s">
-        <v>190</v>
-      </c>
-      <c r="P53" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q53" s="37">
-        <v>6</v>
-      </c>
-      <c r="R53" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="S53" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="T53" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="U53" s="39" t="s">
-        <v>155</v>
-      </c>
-    </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="51" t="s">
+      <c r="A85" s="37" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="51" t="s">
+      <c r="A86" s="37" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="51" t="s">
+      <c r="A87" s="37" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="51" t="s">
+      <c r="A88" s="37" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="51" t="s">
+      <c r="A89" s="37" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="51" t="s">
+      <c r="A90" s="37" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="51" t="s">
+      <c r="A91" s="37" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="51" t="s">
+      <c r="A92" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="51" t="s">
+      <c r="A93" s="37" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="51" t="s">
+      <c r="A94" s="37" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="51" t="s">
+      <c r="A95" s="37" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="51" t="s">
+      <c r="A96" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="51" t="s">
+      <c r="A97" s="37" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="51" t="s">
+      <c r="A98" s="37" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="51" t="s">
+      <c r="A99" s="37" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="51" t="s">
+      <c r="A100" s="37" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="51" t="s">
+      <c r="A101" s="37" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="51" t="s">
+      <c r="A102" s="37" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="51" t="s">
+      <c r="A103" s="37" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="51" t="s">
+      <c r="A104" s="37" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="51" t="s">
+      <c r="A105" s="37" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="51" t="s">
+      <c r="A106" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="51" t="s">
+      <c r="A107" s="37" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="51" t="s">
+      <c r="A108" s="37" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="51" t="s">
+      <c r="A109" s="37" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="51" t="s">
+      <c r="A110" s="37" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="51" t="s">
+      <c r="A111" s="37" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="51" t="s">
+      <c r="A112" s="37" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="51" t="s">
+      <c r="A113" s="37" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="51" t="s">
+      <c r="A114" s="37" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="51" t="s">
+      <c r="A115" s="37" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="51" t="s">
+      <c r="A116" s="37" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="51" t="s">
+      <c r="A117" s="37" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="51" t="s">
+      <c r="A118" s="37" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="51" t="s">
+      <c r="A119" s="37" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="51" t="s">
+      <c r="A120" s="37" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="51" t="s">
+      <c r="A121" s="37" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>